<commit_message>
adding CRUD api for items
</commit_message>
<xml_diff>
--- a/Documentation/Book1.xlsx
+++ b/Documentation/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Groot/Documents/Internship/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Groot/Documents/Internship/Internship/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6623B7CF-E086-934F-93CE-644DAFF441C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B5CE8-CA77-584E-9BA4-CE687AE10ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{6D83E6E5-6B9E-114A-938C-DFBDC887B637}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Requirement  gathering </t>
   </si>
@@ -75,6 +75,33 @@
   </si>
   <si>
     <t>react in frontend and django in backend</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>login/signup</t>
+  </si>
+  <si>
+    <t>homePage</t>
+  </si>
+  <si>
+    <t>product Page</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>10 days</t>
   </si>
 </sst>
 </file>
@@ -118,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,6 +160,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,15 +477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6D0930-017C-8B41-A58C-913D36DE8510}">
-  <dimension ref="D5:I13"/>
+  <dimension ref="C5:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" customWidth="1"/>
     <col min="6" max="6" width="34.5" customWidth="1"/>
     <col min="9" max="9" width="25.1640625" customWidth="1"/>
   </cols>
@@ -528,7 +559,52 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C18:E18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>